<commit_message>
Add Career Profiling engagement tracking to August data sheet - Added column T with flags for users engaged in Career Profiling - Created scripts for data analysis and updates - Updated master Excel file with new engagement tracking column
</commit_message>
<xml_diff>
--- a/August Export_SD 2 Sept_modified.xlsx
+++ b/August Export_SD 2 Sept_modified.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3820" yWindow="760" windowWidth="26780" windowHeight="20400" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="July " sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="August" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet7" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="July " sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="August" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet7" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -10675,7 +10675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R375"/>
+  <dimension ref="A1:T375"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
@@ -10792,6 +10792,11 @@
           <t>USYD Survey 1</t>
         </is>
       </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Career_Profiling_Flag</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -10866,6 +10871,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -10940,6 +10948,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="57" customHeight="1">
       <c r="A4" s="32" t="inlineStr">
@@ -11022,6 +11033,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" ht="57" customHeight="1">
       <c r="A5" s="32" t="inlineStr">
@@ -11096,6 +11110,9 @@
         </is>
       </c>
       <c r="R5" s="37" t="n"/>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" ht="43" customHeight="1">
       <c r="A6" s="32" t="inlineStr">
@@ -11174,6 +11191,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" ht="85" customHeight="1">
       <c r="A7" s="32" t="inlineStr">
@@ -11255,6 +11275,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -11330,6 +11353,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -11400,6 +11426,9 @@
         </is>
       </c>
       <c r="R9" s="7" t="n"/>
+      <c r="T9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" ht="71" customHeight="1">
       <c r="A10" s="32" t="inlineStr">
@@ -11474,6 +11503,9 @@
         </is>
       </c>
       <c r="R10" s="37" t="n"/>
+      <c r="T10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" ht="29" customHeight="1">
       <c r="A11" s="32" t="inlineStr">
@@ -11548,6 +11580,9 @@
         </is>
       </c>
       <c r="R11" s="37" t="n"/>
+      <c r="T11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -11620,6 +11655,9 @@
         </is>
       </c>
       <c r="R12" s="7" t="n"/>
+      <c r="T12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
@@ -11692,6 +11730,9 @@
         </is>
       </c>
       <c r="R13" s="7" t="n"/>
+      <c r="T13" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" ht="29" customHeight="1">
       <c r="A14" s="32" t="inlineStr">
@@ -11770,6 +11811,9 @@
         </is>
       </c>
       <c r="R14" s="37" t="n"/>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
@@ -11838,6 +11882,9 @@
         </is>
       </c>
       <c r="R15" s="7" t="n"/>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="inlineStr">
@@ -11910,6 +11957,9 @@
         </is>
       </c>
       <c r="R16" s="7" t="n"/>
+      <c r="T16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" ht="43" customHeight="1">
       <c r="A17" s="32" t="inlineStr">
@@ -11988,6 +12038,9 @@
         </is>
       </c>
       <c r="R17" s="37" t="n"/>
+      <c r="T17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="32" t="inlineStr">
@@ -12062,6 +12115,9 @@
         </is>
       </c>
       <c r="R18" s="37" t="n"/>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="32" t="inlineStr">
@@ -12134,6 +12190,9 @@
         </is>
       </c>
       <c r="R19" s="37" t="n"/>
+      <c r="T19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" ht="43" customHeight="1">
       <c r="A20" s="32" t="inlineStr">
@@ -12212,6 +12271,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" ht="43" customHeight="1">
       <c r="A21" s="32" t="inlineStr">
@@ -12286,6 +12348,9 @@
         </is>
       </c>
       <c r="R21" s="37" t="n"/>
+      <c r="T21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="32" t="inlineStr">
@@ -12358,6 +12423,9 @@
         </is>
       </c>
       <c r="R22" s="37" t="n"/>
+      <c r="T22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="32" t="inlineStr">
@@ -12432,6 +12500,9 @@
         </is>
       </c>
       <c r="R23" s="37" t="n"/>
+      <c r="T23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" ht="29" customHeight="1">
       <c r="A24" s="32" t="inlineStr">
@@ -12509,6 +12580,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -12584,6 +12658,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T25" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
@@ -12658,6 +12735,9 @@
         </is>
       </c>
       <c r="R26" s="7" t="n"/>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
@@ -12732,6 +12812,9 @@
         </is>
       </c>
       <c r="R27" s="7" t="n"/>
+      <c r="T27" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
@@ -12806,6 +12889,9 @@
         </is>
       </c>
       <c r="R28" s="7" t="n"/>
+      <c r="T28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
@@ -12880,6 +12966,9 @@
         </is>
       </c>
       <c r="R29" s="7" t="n"/>
+      <c r="T29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
@@ -12954,6 +13043,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="32" t="inlineStr">
@@ -13032,6 +13124,9 @@
         </is>
       </c>
       <c r="R31" s="37" t="n"/>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
@@ -13102,6 +13197,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
@@ -13172,6 +13270,9 @@
         </is>
       </c>
       <c r="R33" s="7" t="n"/>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
@@ -13245,6 +13346,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T34" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -13310,6 +13414,9 @@
         </is>
       </c>
       <c r="R35" s="7" t="n"/>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
@@ -13376,6 +13483,9 @@
         </is>
       </c>
       <c r="R36" s="7" t="n"/>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
@@ -13450,6 +13560,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T37" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
@@ -13524,6 +13637,9 @@
         </is>
       </c>
       <c r="R38" s="7" t="n"/>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
@@ -13594,6 +13710,9 @@
         </is>
       </c>
       <c r="R39" s="7" t="n"/>
+      <c r="T39" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
@@ -13668,6 +13787,9 @@
         </is>
       </c>
       <c r="R40" s="7" t="n"/>
+      <c r="T40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" ht="29" customHeight="1">
       <c r="A41" s="32" t="inlineStr">
@@ -13750,6 +13872,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T41" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" ht="29" customHeight="1">
       <c r="A42" s="32" t="inlineStr">
@@ -13828,6 +13953,9 @@
         </is>
       </c>
       <c r="R42" s="37" t="n"/>
+      <c r="T42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" ht="29" customHeight="1">
       <c r="A43" s="32" t="inlineStr">
@@ -13909,6 +14037,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T43" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -13980,6 +14111,9 @@
         </is>
       </c>
       <c r="R44" s="7" t="n"/>
+      <c r="T44" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
@@ -14050,6 +14184,9 @@
         </is>
       </c>
       <c r="R45" s="7" t="n"/>
+      <c r="T45" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" ht="43" customHeight="1">
       <c r="A46" s="32" t="inlineStr">
@@ -14128,6 +14265,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T46" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="32" t="inlineStr">
@@ -14200,6 +14340,9 @@
         </is>
       </c>
       <c r="R47" s="37" t="n"/>
+      <c r="T47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" ht="29" customHeight="1">
       <c r="A48" s="32" t="inlineStr">
@@ -14278,6 +14421,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="32" t="inlineStr">
@@ -14354,6 +14500,9 @@
         </is>
       </c>
       <c r="R49" s="37" t="n"/>
+      <c r="T49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
@@ -14422,6 +14571,9 @@
         </is>
       </c>
       <c r="R50" s="7" t="n"/>
+      <c r="T50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
@@ -14498,6 +14650,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
@@ -14566,6 +14721,9 @@
         </is>
       </c>
       <c r="R52" s="7" t="n"/>
+      <c r="T52" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
@@ -14634,6 +14792,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
@@ -14702,6 +14863,9 @@
         </is>
       </c>
       <c r="R54" s="7" t="n"/>
+      <c r="T54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" ht="29" customHeight="1">
       <c r="A55" s="32" t="inlineStr">
@@ -14780,6 +14944,9 @@
         </is>
       </c>
       <c r="R55" s="37" t="n"/>
+      <c r="T55" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
@@ -14856,6 +15023,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" ht="29" customHeight="1">
       <c r="A57" s="32" t="inlineStr">
@@ -14933,6 +15103,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -15002,6 +15175,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="32" t="inlineStr">
@@ -15076,6 +15252,9 @@
         </is>
       </c>
       <c r="R59" s="37" t="n"/>
+      <c r="T59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="inlineStr">
@@ -15140,6 +15319,9 @@
         </is>
       </c>
       <c r="R60" s="7" t="n"/>
+      <c r="T60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
@@ -15208,6 +15390,9 @@
         </is>
       </c>
       <c r="R61" s="7" t="n"/>
+      <c r="T61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
@@ -15276,6 +15461,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="inlineStr">
@@ -15344,6 +15532,9 @@
         </is>
       </c>
       <c r="R63" s="7" t="n"/>
+      <c r="T63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="inlineStr">
@@ -15418,6 +15609,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" ht="43" customHeight="1">
       <c r="A65" s="32" t="inlineStr">
@@ -15492,6 +15686,9 @@
         </is>
       </c>
       <c r="R65" s="37" t="n"/>
+      <c r="T65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="inlineStr">
@@ -15564,6 +15761,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="32" t="inlineStr">
@@ -15638,6 +15838,9 @@
         </is>
       </c>
       <c r="R67" s="37" t="n"/>
+      <c r="T67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" ht="29" customHeight="1">
       <c r="A68" s="32" t="inlineStr">
@@ -15716,6 +15919,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="32" t="inlineStr">
@@ -15790,6 +15996,9 @@
         </is>
       </c>
       <c r="R69" s="37" t="n"/>
+      <c r="T69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="32" t="inlineStr">
@@ -15864,6 +16073,9 @@
         </is>
       </c>
       <c r="R70" s="37" t="n"/>
+      <c r="T70" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="32" t="inlineStr">
@@ -15938,6 +16150,9 @@
         </is>
       </c>
       <c r="R71" s="37" t="n"/>
+      <c r="T71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" ht="29" customHeight="1">
       <c r="A72" s="32" t="inlineStr">
@@ -16016,6 +16231,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="32" t="inlineStr">
@@ -16088,6 +16306,9 @@
         </is>
       </c>
       <c r="R73" s="37" t="n"/>
+      <c r="T73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="32" t="inlineStr">
@@ -16166,6 +16387,9 @@
         </is>
       </c>
       <c r="R74" s="37" t="n"/>
+      <c r="T74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="32" t="inlineStr">
@@ -16240,6 +16464,9 @@
         </is>
       </c>
       <c r="R75" s="37" t="n"/>
+      <c r="T75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" ht="29" customHeight="1">
       <c r="A76" s="32" t="inlineStr">
@@ -16317,6 +16544,9 @@
         <is>
           <t>I love my degree and have a clear career plan.</t>
         </is>
+      </c>
+      <c r="T76" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -16386,6 +16616,9 @@
         </is>
       </c>
       <c r="R77" s="7" t="n"/>
+      <c r="T77" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" ht="29" customHeight="1">
       <c r="A78" s="32" t="inlineStr">
@@ -16463,6 +16696,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T78" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="79">
@@ -16536,6 +16772,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="32" t="inlineStr">
@@ -16610,6 +16849,9 @@
         </is>
       </c>
       <c r="R80" s="37" t="n"/>
+      <c r="T80" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="81" ht="43" customHeight="1">
       <c r="A81" s="32" t="inlineStr">
@@ -16692,6 +16934,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T81" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="32" t="inlineStr">
@@ -16766,6 +17011,9 @@
         </is>
       </c>
       <c r="R82" s="37" t="n"/>
+      <c r="T82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" ht="43" customHeight="1">
       <c r="A83" s="32" t="inlineStr">
@@ -16848,6 +17096,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="32" t="inlineStr">
@@ -16920,6 +17171,9 @@
         </is>
       </c>
       <c r="R84" s="37" t="n"/>
+      <c r="T84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="32" t="inlineStr">
@@ -16994,6 +17248,9 @@
         </is>
       </c>
       <c r="R85" s="37" t="n"/>
+      <c r="T85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="inlineStr">
@@ -17066,6 +17323,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T86" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="inlineStr">
@@ -17134,6 +17394,9 @@
         </is>
       </c>
       <c r="R87" s="7" t="n"/>
+      <c r="T87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="32" t="inlineStr">
@@ -17206,6 +17469,9 @@
         </is>
       </c>
       <c r="R88" s="37" t="n"/>
+      <c r="T88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="32" t="inlineStr">
@@ -17280,6 +17546,9 @@
         </is>
       </c>
       <c r="R89" s="37" t="n"/>
+      <c r="T89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="32" t="inlineStr">
@@ -17354,6 +17623,9 @@
         </is>
       </c>
       <c r="R90" s="37" t="n"/>
+      <c r="T90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="32" t="inlineStr">
@@ -17430,6 +17702,9 @@
         </is>
       </c>
       <c r="R91" s="37" t="n"/>
+      <c r="T91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="32" t="inlineStr">
@@ -17504,6 +17779,9 @@
         </is>
       </c>
       <c r="R92" s="37" t="n"/>
+      <c r="T92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="32" t="inlineStr">
@@ -17578,6 +17856,9 @@
         </is>
       </c>
       <c r="R93" s="37" t="n"/>
+      <c r="T93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="32" t="inlineStr">
@@ -17655,6 +17936,9 @@
         <is>
           <t>I feel lost - I don't think my degree is right for me.</t>
         </is>
+      </c>
+      <c r="T94" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -17732,6 +18016,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T95" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="32" t="inlineStr">
@@ -17806,6 +18093,9 @@
         </is>
       </c>
       <c r="R96" s="37" t="n"/>
+      <c r="T96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" ht="29" customHeight="1">
       <c r="A97" s="32" t="inlineStr">
@@ -17883,6 +18173,9 @@
         <is>
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
+      </c>
+      <c r="T97" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -17956,6 +18249,9 @@
         </is>
       </c>
       <c r="R98" s="7" t="n"/>
+      <c r="T98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="32" t="inlineStr">
@@ -18030,6 +18326,9 @@
         </is>
       </c>
       <c r="R99" s="37" t="n"/>
+      <c r="T99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="inlineStr">
@@ -18098,6 +18397,9 @@
         </is>
       </c>
       <c r="R100" s="7" t="n"/>
+      <c r="T100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="32" t="inlineStr">
@@ -18174,6 +18476,9 @@
         </is>
       </c>
       <c r="R101" s="37" t="n"/>
+      <c r="T101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" ht="43" customHeight="1">
       <c r="A102" s="32" t="inlineStr">
@@ -18255,6 +18560,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T102" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -18328,6 +18636,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="32" t="inlineStr">
@@ -18402,6 +18713,9 @@
         </is>
       </c>
       <c r="R104" s="37" t="n"/>
+      <c r="T104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="32" t="inlineStr">
@@ -18470,6 +18784,9 @@
         </is>
       </c>
       <c r="R105" s="37" t="n"/>
+      <c r="T105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" ht="29" customHeight="1">
       <c r="A106" s="32" t="inlineStr">
@@ -18551,6 +18868,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T106" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -18596,6 +18916,9 @@
       <c r="P107" s="24" t="n"/>
       <c r="Q107" s="24" t="n"/>
       <c r="R107" s="7" t="n"/>
+      <c r="T107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" ht="29" customHeight="1">
       <c r="A108" s="32" t="inlineStr">
@@ -18652,6 +18975,9 @@
       <c r="P108" s="41" t="n"/>
       <c r="Q108" s="41" t="n"/>
       <c r="R108" s="37" t="n"/>
+      <c r="T108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="inlineStr">
@@ -18696,6 +19022,9 @@
       <c r="P109" s="24" t="n"/>
       <c r="Q109" s="24" t="n"/>
       <c r="R109" s="7" t="n"/>
+      <c r="T109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="32" t="inlineStr">
@@ -18748,6 +19077,9 @@
       <c r="P110" s="41" t="n"/>
       <c r="Q110" s="41" t="n"/>
       <c r="R110" s="37" t="n"/>
+      <c r="T110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="32" t="inlineStr">
@@ -18800,6 +19132,9 @@
       <c r="P111" s="41" t="n"/>
       <c r="Q111" s="41" t="n"/>
       <c r="R111" s="37" t="n"/>
+      <c r="T111" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="inlineStr">
@@ -18844,6 +19179,9 @@
       <c r="P112" s="24" t="n"/>
       <c r="Q112" s="24" t="n"/>
       <c r="R112" s="7" t="n"/>
+      <c r="T112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="32" t="inlineStr">
@@ -18896,6 +19234,9 @@
       <c r="P113" s="41" t="n"/>
       <c r="Q113" s="41" t="n"/>
       <c r="R113" s="37" t="n"/>
+      <c r="T113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="32" t="inlineStr">
@@ -18948,6 +19289,9 @@
       <c r="P114" s="41" t="n"/>
       <c r="Q114" s="41" t="n"/>
       <c r="R114" s="37" t="n"/>
+      <c r="T114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="32" t="inlineStr">
@@ -19000,6 +19344,9 @@
       <c r="P115" s="41" t="n"/>
       <c r="Q115" s="41" t="n"/>
       <c r="R115" s="37" t="n"/>
+      <c r="T115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="32" t="inlineStr">
@@ -19052,6 +19399,9 @@
       <c r="P116" s="41" t="n"/>
       <c r="Q116" s="41" t="n"/>
       <c r="R116" s="37" t="n"/>
+      <c r="T116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="32" t="inlineStr">
@@ -19100,6 +19450,9 @@
       <c r="P117" s="41" t="n"/>
       <c r="Q117" s="41" t="n"/>
       <c r="R117" s="37" t="n"/>
+      <c r="T117" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="inlineStr">
@@ -19168,6 +19521,9 @@
         </is>
       </c>
       <c r="R118" s="7" t="n"/>
+      <c r="T118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" ht="43" customHeight="1">
       <c r="A119" s="32" t="inlineStr">
@@ -19250,6 +19606,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T119" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" ht="43" customHeight="1">
       <c r="A120" s="32" t="inlineStr">
@@ -19327,6 +19686,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T120" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -19396,6 +19758,9 @@
         </is>
       </c>
       <c r="R121" s="7" t="n"/>
+      <c r="T121" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="inlineStr">
@@ -19472,6 +19837,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T122" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="inlineStr">
@@ -19544,6 +19912,9 @@
         </is>
       </c>
       <c r="R123" s="7" t="n"/>
+      <c r="T123" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="inlineStr">
@@ -19616,6 +19987,9 @@
         </is>
       </c>
       <c r="R124" s="7" t="n"/>
+      <c r="T124" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="inlineStr">
@@ -19688,6 +20062,9 @@
         </is>
       </c>
       <c r="R125" s="7" t="n"/>
+      <c r="T125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="inlineStr">
@@ -19760,6 +20137,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="inlineStr">
@@ -19832,6 +20212,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T127" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="inlineStr">
@@ -19904,6 +20287,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T128" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="inlineStr">
@@ -19972,6 +20358,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T129" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="inlineStr">
@@ -20044,6 +20433,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T130" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="inlineStr">
@@ -20112,6 +20504,9 @@
         </is>
       </c>
       <c r="R131" s="7" t="n"/>
+      <c r="T131" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="132" ht="29" customHeight="1">
       <c r="A132" s="32" t="inlineStr">
@@ -20193,6 +20588,9 @@
         <is>
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
+      </c>
+      <c r="T132" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -20266,6 +20664,9 @@
         </is>
       </c>
       <c r="R133" s="7" t="n"/>
+      <c r="T133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="inlineStr">
@@ -20334,6 +20735,9 @@
         </is>
       </c>
       <c r="R134" s="7" t="n"/>
+      <c r="T134" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="inlineStr">
@@ -20406,6 +20810,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T135" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="inlineStr">
@@ -20474,6 +20881,9 @@
         </is>
       </c>
       <c r="R136" s="7" t="n"/>
+      <c r="T136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" ht="29" customHeight="1">
       <c r="A137" s="32" t="inlineStr">
@@ -20555,6 +20965,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T137" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -20628,6 +21041,9 @@
         </is>
       </c>
       <c r="R138" s="7" t="n"/>
+      <c r="T138" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" ht="57" customHeight="1">
       <c r="A139" s="32" t="inlineStr">
@@ -20706,6 +21122,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T139" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" ht="57" customHeight="1">
       <c r="A140" s="32" t="inlineStr">
@@ -20783,6 +21202,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T140" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="141">
@@ -20856,6 +21278,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T141" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="inlineStr">
@@ -20926,6 +21351,9 @@
         </is>
       </c>
       <c r="R142" s="7" t="n"/>
+      <c r="T142" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="32" t="inlineStr">
@@ -21004,6 +21432,9 @@
         </is>
       </c>
       <c r="R143" s="37" t="n"/>
+      <c r="T143" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="inlineStr">
@@ -21074,6 +21505,9 @@
         </is>
       </c>
       <c r="R144" s="7" t="n"/>
+      <c r="T144" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="inlineStr">
@@ -21142,6 +21576,9 @@
         </is>
       </c>
       <c r="R145" s="7" t="n"/>
+      <c r="T145" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="inlineStr">
@@ -21212,6 +21649,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T146" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="inlineStr">
@@ -21282,6 +21722,9 @@
         </is>
       </c>
       <c r="R147" s="7" t="n"/>
+      <c r="T147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="inlineStr">
@@ -21356,6 +21799,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T148" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="inlineStr">
@@ -21434,6 +21880,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T149" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="inlineStr">
@@ -21508,6 +21957,9 @@
           <t>I feel lost - I don't think my degree is right for me.</t>
         </is>
       </c>
+      <c r="T150" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="inlineStr">
@@ -21574,6 +22026,9 @@
         </is>
       </c>
       <c r="R151" s="7" t="n"/>
+      <c r="T151" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="32" t="inlineStr">
@@ -21652,6 +22107,9 @@
         </is>
       </c>
       <c r="R152" s="37" t="n"/>
+      <c r="T152" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="inlineStr">
@@ -21716,6 +22174,9 @@
         </is>
       </c>
       <c r="R153" s="7" t="n"/>
+      <c r="T153" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" ht="57" customHeight="1">
       <c r="A154" s="32" t="inlineStr">
@@ -21797,6 +22258,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T154" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -21870,6 +22334,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T155" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" ht="29" customHeight="1">
       <c r="A156" s="32" t="inlineStr">
@@ -21944,6 +22411,9 @@
         </is>
       </c>
       <c r="R156" s="37" t="n"/>
+      <c r="T156" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" ht="29" customHeight="1">
       <c r="A157" s="32" t="inlineStr">
@@ -22020,6 +22490,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T157" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" ht="43" customHeight="1">
       <c r="A158" s="32" t="inlineStr">
@@ -22097,6 +22570,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T158" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -22162,6 +22638,9 @@
         </is>
       </c>
       <c r="R159" s="7" t="n"/>
+      <c r="T159" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="inlineStr">
@@ -22234,6 +22713,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T160" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="inlineStr">
@@ -22306,6 +22788,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T161" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="inlineStr">
@@ -22380,6 +22865,9 @@
         </is>
       </c>
       <c r="R162" s="7" t="n"/>
+      <c r="T162" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="inlineStr">
@@ -22453,6 +22941,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T163" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -22526,6 +23017,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T164" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="inlineStr">
@@ -22600,6 +23094,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T165" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="inlineStr">
@@ -22670,6 +23167,9 @@
         </is>
       </c>
       <c r="R166" s="7" t="n"/>
+      <c r="T166" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="inlineStr">
@@ -22744,6 +23244,9 @@
         </is>
       </c>
       <c r="R167" s="7" t="n"/>
+      <c r="T167" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="inlineStr">
@@ -22822,6 +23325,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T168" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="inlineStr">
@@ -22896,6 +23402,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T169" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="inlineStr">
@@ -22970,6 +23479,9 @@
         </is>
       </c>
       <c r="R170" s="7" t="n"/>
+      <c r="T170" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="inlineStr">
@@ -23044,6 +23556,9 @@
         </is>
       </c>
       <c r="R171" s="7" t="n"/>
+      <c r="T171" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="inlineStr">
@@ -23114,6 +23629,9 @@
         </is>
       </c>
       <c r="R172" s="7" t="n"/>
+      <c r="T172" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="inlineStr">
@@ -23184,6 +23702,9 @@
         </is>
       </c>
       <c r="R173" s="7" t="n"/>
+      <c r="T173" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="inlineStr">
@@ -23254,6 +23775,9 @@
         </is>
       </c>
       <c r="R174" s="7" t="n"/>
+      <c r="T174" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="inlineStr">
@@ -23328,6 +23852,9 @@
         </is>
       </c>
       <c r="R175" s="7" t="n"/>
+      <c r="T175" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="inlineStr">
@@ -23394,6 +23921,9 @@
         </is>
       </c>
       <c r="R176" s="7" t="n"/>
+      <c r="T176" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="inlineStr">
@@ -23468,6 +23998,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T177" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178" ht="57" customHeight="1">
       <c r="A178" s="32" t="inlineStr">
@@ -23547,6 +24080,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T178" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -23616,6 +24152,9 @@
         </is>
       </c>
       <c r="R179" s="7" t="n"/>
+      <c r="T179" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="inlineStr">
@@ -23688,6 +24227,9 @@
         </is>
       </c>
       <c r="R180" s="7" t="n"/>
+      <c r="T180" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="inlineStr">
@@ -23756,6 +24298,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T181" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="inlineStr">
@@ -23828,6 +24373,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T182" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="inlineStr">
@@ -23900,6 +24448,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T183" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184" ht="29" customHeight="1">
       <c r="A184" s="32" t="inlineStr">
@@ -23977,6 +24528,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T184" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -24042,6 +24596,9 @@
         </is>
       </c>
       <c r="R185" s="7" t="n"/>
+      <c r="T185" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="inlineStr">
@@ -24106,6 +24663,9 @@
         </is>
       </c>
       <c r="R186" s="7" t="n"/>
+      <c r="T186" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="187" ht="29" customHeight="1">
       <c r="A187" s="32" t="inlineStr">
@@ -24183,6 +24743,9 @@
         <is>
           <t>I love my degree and have a clear career plan.</t>
         </is>
+      </c>
+      <c r="T187" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -24248,6 +24811,9 @@
         </is>
       </c>
       <c r="R188" s="7" t="n"/>
+      <c r="T188" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="inlineStr">
@@ -24316,6 +24882,9 @@
         </is>
       </c>
       <c r="R189" s="7" t="n"/>
+      <c r="T189" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="inlineStr">
@@ -24384,6 +24953,9 @@
         </is>
       </c>
       <c r="R190" s="7" t="n"/>
+      <c r="T190" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="32" t="inlineStr">
@@ -24456,6 +25028,9 @@
         </is>
       </c>
       <c r="R191" s="37" t="n"/>
+      <c r="T191" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="inlineStr">
@@ -24520,6 +25095,9 @@
         </is>
       </c>
       <c r="R192" s="7" t="n"/>
+      <c r="T192" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="inlineStr">
@@ -24588,6 +25166,9 @@
         </is>
       </c>
       <c r="R193" s="7" t="n"/>
+      <c r="T193" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="inlineStr">
@@ -24656,6 +25237,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T194" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="2" t="inlineStr">
@@ -24724,6 +25308,9 @@
         </is>
       </c>
       <c r="R195" s="7" t="n"/>
+      <c r="T195" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="2" t="inlineStr">
@@ -24800,6 +25387,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T196" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="197" ht="29" customHeight="1">
       <c r="A197" s="32" t="inlineStr">
@@ -24877,6 +25467,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T197" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -24950,6 +25543,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T198" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="2" t="inlineStr">
@@ -25018,6 +25614,9 @@
         </is>
       </c>
       <c r="R199" s="7" t="n"/>
+      <c r="T199" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="2" t="inlineStr">
@@ -25082,6 +25681,9 @@
         </is>
       </c>
       <c r="R200" s="7" t="n"/>
+      <c r="T200" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="32" t="inlineStr">
@@ -25156,6 +25758,9 @@
         </is>
       </c>
       <c r="R201" s="37" t="n"/>
+      <c r="T201" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="inlineStr">
@@ -25224,6 +25829,9 @@
         </is>
       </c>
       <c r="R202" s="7" t="n"/>
+      <c r="T202" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="32" t="inlineStr">
@@ -25298,6 +25906,9 @@
         </is>
       </c>
       <c r="R203" s="37" t="n"/>
+      <c r="T203" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="32" t="inlineStr">
@@ -25372,6 +25983,9 @@
         </is>
       </c>
       <c r="R204" s="37" t="n"/>
+      <c r="T204" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="32" t="inlineStr">
@@ -25444,6 +26058,9 @@
         </is>
       </c>
       <c r="R205" s="37" t="n"/>
+      <c r="T205" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="32" t="inlineStr">
@@ -25516,6 +26133,9 @@
         </is>
       </c>
       <c r="R206" s="37" t="n"/>
+      <c r="T206" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="inlineStr">
@@ -25580,6 +26200,9 @@
         </is>
       </c>
       <c r="R207" s="7" t="n"/>
+      <c r="T207" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="32" t="inlineStr">
@@ -25654,6 +26277,9 @@
         </is>
       </c>
       <c r="R208" s="37" t="n"/>
+      <c r="T208" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="2" t="inlineStr">
@@ -25724,6 +26350,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T209" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="inlineStr">
@@ -25802,6 +26431,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T210" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="inlineStr">
@@ -25876,6 +26508,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T211" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="inlineStr">
@@ -25950,6 +26585,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T212" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="inlineStr">
@@ -26020,6 +26658,9 @@
         </is>
       </c>
       <c r="R213" s="7" t="n"/>
+      <c r="T213" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="inlineStr">
@@ -26090,6 +26731,9 @@
         </is>
       </c>
       <c r="R214" s="7" t="n"/>
+      <c r="T214" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="215" ht="29" customHeight="1">
       <c r="A215" s="32" t="inlineStr">
@@ -26166,6 +26810,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T215" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="216" ht="43" customHeight="1">
       <c r="A216" s="32" t="inlineStr">
@@ -26243,6 +26890,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T216" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="217">
@@ -26316,6 +26966,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T217" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="inlineStr">
@@ -26380,6 +27033,9 @@
         </is>
       </c>
       <c r="R218" s="7" t="n"/>
+      <c r="T218" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="32" t="inlineStr">
@@ -26446,6 +27102,9 @@
       </c>
       <c r="Q219" s="41" t="n"/>
       <c r="R219" s="37" t="n"/>
+      <c r="T219" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="220" ht="29" customHeight="1">
       <c r="A220" s="32" t="inlineStr">
@@ -26527,6 +27186,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T220" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -26594,6 +27256,9 @@
         </is>
       </c>
       <c r="R221" s="7" t="n"/>
+      <c r="T221" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="inlineStr">
@@ -26667,6 +27332,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T222" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -26740,6 +27408,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T223" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="inlineStr">
@@ -26806,6 +27477,9 @@
         </is>
       </c>
       <c r="R224" s="7" t="n"/>
+      <c r="T224" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="225" ht="43" customHeight="1">
       <c r="A225" s="32" t="inlineStr">
@@ -26885,6 +27559,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T225" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="226">
@@ -26960,6 +27637,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T226" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="inlineStr">
@@ -27026,6 +27706,9 @@
         </is>
       </c>
       <c r="R227" s="7" t="n"/>
+      <c r="T227" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="inlineStr">
@@ -27092,6 +27775,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T228" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="2" t="inlineStr">
@@ -27162,6 +27848,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T229" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="inlineStr">
@@ -27236,6 +27925,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T230" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="231" ht="29" customHeight="1">
       <c r="A231" s="32" t="inlineStr">
@@ -27313,6 +28005,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T231" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="232">
@@ -27384,6 +28079,9 @@
         </is>
       </c>
       <c r="R232" s="7" t="n"/>
+      <c r="T232" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="inlineStr">
@@ -27458,6 +28156,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T233" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="32" t="inlineStr">
@@ -27532,6 +28233,9 @@
         </is>
       </c>
       <c r="R234" s="37" t="n"/>
+      <c r="T234" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="235" ht="43" customHeight="1">
       <c r="A235" s="32" t="inlineStr">
@@ -27613,6 +28317,9 @@
         <is>
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
+      </c>
+      <c r="T235" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -27682,6 +28389,9 @@
         </is>
       </c>
       <c r="R236" s="7" t="n"/>
+      <c r="T236" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="2" t="inlineStr">
@@ -27754,6 +28464,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T237" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="inlineStr">
@@ -27822,6 +28535,9 @@
         </is>
       </c>
       <c r="R238" s="7" t="n"/>
+      <c r="T238" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="inlineStr">
@@ -27894,6 +28610,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T239" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="32" t="inlineStr">
@@ -27968,6 +28687,9 @@
         </is>
       </c>
       <c r="R240" s="37" t="n"/>
+      <c r="T240" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="2" t="inlineStr">
@@ -28036,6 +28758,9 @@
         </is>
       </c>
       <c r="R241" s="7" t="n"/>
+      <c r="T241" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="inlineStr">
@@ -28100,6 +28825,9 @@
         </is>
       </c>
       <c r="R242" s="7" t="n"/>
+      <c r="T242" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="2" t="inlineStr">
@@ -28168,6 +28896,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T243" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" ht="29" customHeight="1">
       <c r="A244" s="32" t="inlineStr">
@@ -28246,6 +28977,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T244" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="245" ht="29" customHeight="1">
       <c r="A245" s="32" t="inlineStr">
@@ -28323,6 +29057,9 @@
         <is>
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
+      </c>
+      <c r="T245" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -28392,6 +29129,9 @@
         </is>
       </c>
       <c r="R246" s="7" t="n"/>
+      <c r="T246" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="2" t="inlineStr">
@@ -28464,6 +29204,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T247" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="2" t="inlineStr">
@@ -28536,6 +29279,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T248" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="2" t="inlineStr">
@@ -28604,6 +29350,9 @@
         </is>
       </c>
       <c r="R249" s="7" t="n"/>
+      <c r="T249" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="32" t="inlineStr">
@@ -28678,6 +29427,9 @@
         </is>
       </c>
       <c r="R250" s="37" t="n"/>
+      <c r="T250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="2" t="inlineStr">
@@ -28750,6 +29502,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T251" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="2" t="inlineStr">
@@ -28814,6 +29569,9 @@
         </is>
       </c>
       <c r="R252" s="7" t="n"/>
+      <c r="T252" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="2" t="inlineStr">
@@ -28888,6 +29646,9 @@
         </is>
       </c>
       <c r="R253" s="7" t="n"/>
+      <c r="T253" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="2" t="inlineStr">
@@ -28966,6 +29727,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T254" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="2" t="inlineStr">
@@ -29036,6 +29800,9 @@
         </is>
       </c>
       <c r="R255" s="7" t="n"/>
+      <c r="T255" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="2" t="inlineStr">
@@ -29110,6 +29877,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T256" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="2" t="inlineStr">
@@ -29184,6 +29954,9 @@
         </is>
       </c>
       <c r="R257" s="7" t="n"/>
+      <c r="T257" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="2" t="inlineStr">
@@ -29258,6 +30031,9 @@
         </is>
       </c>
       <c r="R258" s="7" t="n"/>
+      <c r="T258" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="2" t="inlineStr">
@@ -29327,6 +30103,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T259" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="260">
@@ -29392,6 +30171,9 @@
         </is>
       </c>
       <c r="R260" s="7" t="n"/>
+      <c r="T260" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="2" t="inlineStr">
@@ -29464,6 +30246,9 @@
         </is>
       </c>
       <c r="R261" s="7" t="n"/>
+      <c r="T261" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="2" t="inlineStr">
@@ -29536,6 +30321,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T262" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="2" t="inlineStr">
@@ -29604,6 +30392,9 @@
         </is>
       </c>
       <c r="R263" s="7" t="n"/>
+      <c r="T263" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="32" t="inlineStr">
@@ -29678,6 +30469,9 @@
         </is>
       </c>
       <c r="R264" s="37" t="n"/>
+      <c r="T264" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="2" t="inlineStr">
@@ -29742,6 +30536,9 @@
         </is>
       </c>
       <c r="R265" s="7" t="n"/>
+      <c r="T265" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="2" t="inlineStr">
@@ -29810,6 +30607,9 @@
         </is>
       </c>
       <c r="R266" s="7" t="n"/>
+      <c r="T266" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="2" t="inlineStr">
@@ -29884,6 +30684,9 @@
         </is>
       </c>
       <c r="R267" s="7" t="n"/>
+      <c r="T267" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="2" t="inlineStr">
@@ -29954,6 +30757,9 @@
         </is>
       </c>
       <c r="R268" s="7" t="n"/>
+      <c r="T268" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="2" t="inlineStr">
@@ -30027,6 +30833,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T269" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="270">
@@ -30100,6 +30909,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T270" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="33" t="inlineStr">
@@ -30172,6 +30984,9 @@
         </is>
       </c>
       <c r="R271" s="37" t="n"/>
+      <c r="T271" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="27" t="inlineStr">
@@ -30242,6 +31057,9 @@
         </is>
       </c>
       <c r="R272" s="29" t="n"/>
+      <c r="T272" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="39" t="inlineStr">
@@ -30316,6 +31134,9 @@
         </is>
       </c>
       <c r="R273" s="41" t="n"/>
+      <c r="T273" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="274" ht="29" customHeight="1">
       <c r="A274" s="39" t="inlineStr">
@@ -30390,6 +31211,9 @@
         </is>
       </c>
       <c r="R274" s="41" t="n"/>
+      <c r="T274" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="39" t="inlineStr">
@@ -30464,6 +31288,9 @@
         </is>
       </c>
       <c r="R275" s="41" t="n"/>
+      <c r="T275" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="27" t="inlineStr">
@@ -30532,6 +31359,9 @@
         </is>
       </c>
       <c r="R276" s="29" t="n"/>
+      <c r="T276" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="27" t="inlineStr">
@@ -30600,6 +31430,9 @@
         </is>
       </c>
       <c r="R277" s="29" t="n"/>
+      <c r="T277" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="27" t="inlineStr">
@@ -30664,6 +31497,9 @@
         </is>
       </c>
       <c r="R278" s="29" t="n"/>
+      <c r="T278" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="39" t="inlineStr">
@@ -30736,6 +31572,9 @@
         </is>
       </c>
       <c r="R279" s="41" t="n"/>
+      <c r="T279" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="27" t="inlineStr">
@@ -30800,6 +31639,9 @@
         </is>
       </c>
       <c r="R280" s="29" t="n"/>
+      <c r="T280" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="39" t="inlineStr">
@@ -30874,6 +31716,9 @@
         </is>
       </c>
       <c r="R281" s="41" t="n"/>
+      <c r="T281" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="282" ht="29" customHeight="1">
       <c r="A282" s="39" t="inlineStr">
@@ -30955,6 +31800,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T282" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="283">
@@ -31028,6 +31876,9 @@
         </is>
       </c>
       <c r="R283" s="29" t="n"/>
+      <c r="T283" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="27" t="inlineStr">
@@ -31096,6 +31947,9 @@
         </is>
       </c>
       <c r="R284" s="29" t="n"/>
+      <c r="T284" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="39" t="inlineStr">
@@ -31170,6 +32024,9 @@
         </is>
       </c>
       <c r="R285" s="41" t="n"/>
+      <c r="T285" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="27" t="inlineStr">
@@ -31234,6 +32091,9 @@
         </is>
       </c>
       <c r="R286" s="29" t="n"/>
+      <c r="T286" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="27" t="inlineStr">
@@ -31298,6 +32158,9 @@
         </is>
       </c>
       <c r="R287" s="29" t="n"/>
+      <c r="T287" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="27" t="inlineStr">
@@ -31366,6 +32229,9 @@
         </is>
       </c>
       <c r="R288" s="29" t="n"/>
+      <c r="T288" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="27" t="inlineStr">
@@ -31434,6 +32300,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T289" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="39" t="inlineStr">
@@ -31511,6 +32380,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T290" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="291">
@@ -31584,6 +32456,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T291" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="27" t="inlineStr">
@@ -31660,6 +32535,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T292" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="39" t="inlineStr">
@@ -31734,6 +32612,9 @@
         </is>
       </c>
       <c r="R293" s="41" t="n"/>
+      <c r="T293" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="27" t="inlineStr">
@@ -31806,6 +32687,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T294" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="27" t="inlineStr">
@@ -31874,6 +32758,9 @@
         </is>
       </c>
       <c r="R295" s="29" t="n"/>
+      <c r="T295" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="39" t="inlineStr">
@@ -31948,6 +32835,9 @@
         </is>
       </c>
       <c r="R296" s="41" t="n"/>
+      <c r="T296" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="27" t="inlineStr">
@@ -32016,6 +32906,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T297" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="27" t="inlineStr">
@@ -32088,6 +32981,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T298" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="27" t="inlineStr">
@@ -32152,6 +33048,9 @@
       </c>
       <c r="Q299" s="24" t="n"/>
       <c r="R299" s="29" t="n"/>
+      <c r="T299" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="27" t="inlineStr">
@@ -32228,6 +33127,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T300" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="27" t="inlineStr">
@@ -32292,6 +33194,9 @@
         </is>
       </c>
       <c r="R301" s="29" t="n"/>
+      <c r="T301" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="39" t="inlineStr">
@@ -32366,6 +33271,9 @@
         </is>
       </c>
       <c r="R302" s="41" t="n"/>
+      <c r="T302" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="39" t="inlineStr">
@@ -32440,6 +33348,9 @@
         </is>
       </c>
       <c r="R303" s="41" t="n"/>
+      <c r="T303" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="27" t="inlineStr">
@@ -32516,6 +33427,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T304" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="27" t="inlineStr">
@@ -32584,6 +33498,9 @@
         </is>
       </c>
       <c r="R305" s="29" t="n"/>
+      <c r="T305" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="39" t="inlineStr">
@@ -32658,6 +33575,9 @@
         </is>
       </c>
       <c r="R306" s="41" t="n"/>
+      <c r="T306" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="307" ht="43" customHeight="1">
       <c r="A307" s="39" t="inlineStr">
@@ -32735,6 +33655,9 @@
         <is>
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
+      </c>
+      <c r="T307" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="308">
@@ -32804,6 +33727,9 @@
         </is>
       </c>
       <c r="R308" s="29" t="n"/>
+      <c r="T308" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="27" t="inlineStr">
@@ -32872,6 +33798,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T309" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="27" t="inlineStr">
@@ -32944,6 +33873,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T310" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="311" ht="43" customHeight="1">
       <c r="A311" s="39" t="inlineStr">
@@ -33027,6 +33959,9 @@
         <is>
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
+      </c>
+      <c r="T311" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="312">
@@ -33102,6 +34037,9 @@
         </is>
       </c>
       <c r="R312" s="29" t="n"/>
+      <c r="T312" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="27" t="inlineStr">
@@ -33172,6 +34110,9 @@
         </is>
       </c>
       <c r="R313" s="29" t="n"/>
+      <c r="T313" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="27" t="inlineStr">
@@ -33242,6 +34183,9 @@
         </is>
       </c>
       <c r="R314" s="29" t="n"/>
+      <c r="T314" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="27" t="inlineStr">
@@ -33312,6 +34256,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T315" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="27" t="inlineStr">
@@ -33382,6 +34329,9 @@
         </is>
       </c>
       <c r="R316" s="29" t="n"/>
+      <c r="T316" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="27" t="inlineStr">
@@ -33456,6 +34406,9 @@
         </is>
       </c>
       <c r="R317" s="29" t="n"/>
+      <c r="T317" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="27" t="inlineStr">
@@ -33522,6 +34475,9 @@
         </is>
       </c>
       <c r="R318" s="29" t="n"/>
+      <c r="T318" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="27" t="inlineStr">
@@ -33598,6 +34554,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T319" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="27" t="inlineStr">
@@ -33672,6 +34631,9 @@
         </is>
       </c>
       <c r="R320" s="29" t="n"/>
+      <c r="T320" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="27" t="inlineStr">
@@ -33746,6 +34708,9 @@
         </is>
       </c>
       <c r="R321" s="29" t="n"/>
+      <c r="T321" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="27" t="inlineStr">
@@ -33824,6 +34789,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T322" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="27" t="inlineStr">
@@ -33894,6 +34862,9 @@
         </is>
       </c>
       <c r="R323" s="29" t="n"/>
+      <c r="T323" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="27" t="inlineStr">
@@ -33964,6 +34935,9 @@
         </is>
       </c>
       <c r="R324" s="29" t="n"/>
+      <c r="T324" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="27" t="inlineStr">
@@ -34038,6 +35012,9 @@
         </is>
       </c>
       <c r="R325" s="29" t="n"/>
+      <c r="T325" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="27" t="inlineStr">
@@ -34112,6 +35089,9 @@
         </is>
       </c>
       <c r="R326" s="29" t="n"/>
+      <c r="T326" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="27" t="inlineStr">
@@ -34180,6 +35160,9 @@
         </is>
       </c>
       <c r="R327" s="29" t="n"/>
+      <c r="T327" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="27" t="inlineStr">
@@ -34250,6 +35233,9 @@
         </is>
       </c>
       <c r="R328" s="29" t="n"/>
+      <c r="T328" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="27" t="inlineStr">
@@ -34320,6 +35306,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T329" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="27" t="inlineStr">
@@ -34398,6 +35387,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T330" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="27" t="inlineStr">
@@ -34472,6 +35464,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T331" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="27" t="inlineStr">
@@ -34550,6 +35545,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T332" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="27" t="inlineStr">
@@ -34624,6 +35622,9 @@
         </is>
       </c>
       <c r="R333" s="29" t="n"/>
+      <c r="T333" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="27" t="inlineStr">
@@ -34692,6 +35693,9 @@
         </is>
       </c>
       <c r="R334" s="29" t="n"/>
+      <c r="T334" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="27" t="inlineStr">
@@ -34766,6 +35770,9 @@
         </is>
       </c>
       <c r="R335" s="29" t="n"/>
+      <c r="T335" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="27" t="inlineStr">
@@ -34844,6 +35851,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T336" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="27" t="inlineStr">
@@ -34910,6 +35920,9 @@
         </is>
       </c>
       <c r="R337" s="29" t="n"/>
+      <c r="T337" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="27" t="inlineStr">
@@ -34984,6 +35997,9 @@
         </is>
       </c>
       <c r="R338" s="29" t="n"/>
+      <c r="T338" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="27" t="inlineStr">
@@ -35058,6 +36074,9 @@
         </is>
       </c>
       <c r="R339" s="29" t="n"/>
+      <c r="T339" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="27" t="inlineStr">
@@ -35106,6 +36125,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T340" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="27" t="inlineStr">
@@ -35150,6 +36172,9 @@
       <c r="P341" s="24" t="n"/>
       <c r="Q341" s="24" t="n"/>
       <c r="R341" s="29" t="n"/>
+      <c r="T341" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="27" t="inlineStr">
@@ -35198,6 +36223,9 @@
           <t>I love my degree and have a clear career plan.</t>
         </is>
       </c>
+      <c r="T342" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="27" t="inlineStr">
@@ -35242,6 +36270,9 @@
       <c r="P343" s="24" t="n"/>
       <c r="Q343" s="24" t="n"/>
       <c r="R343" s="29" t="n"/>
+      <c r="T343" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="39" t="inlineStr">
@@ -35300,6 +36331,9 @@
       <c r="P344" s="41" t="n"/>
       <c r="Q344" s="41" t="n"/>
       <c r="R344" s="41" t="n"/>
+      <c r="T344" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="39" t="inlineStr">
@@ -35358,6 +36392,9 @@
       <c r="P345" s="41" t="n"/>
       <c r="Q345" s="41" t="n"/>
       <c r="R345" s="41" t="n"/>
+      <c r="T345" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="39" t="inlineStr">
@@ -35410,6 +36447,9 @@
       <c r="P346" s="41" t="n"/>
       <c r="Q346" s="41" t="n"/>
       <c r="R346" s="41" t="n"/>
+      <c r="T346" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="27" t="inlineStr">
@@ -35458,6 +36498,9 @@
           <t>I'm enjoying my studies and have some ideas for my career.</t>
         </is>
       </c>
+      <c r="T347" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="27" t="inlineStr">
@@ -35502,6 +36545,9 @@
       <c r="P348" s="24" t="n"/>
       <c r="Q348" s="24" t="n"/>
       <c r="R348" s="29" t="n"/>
+      <c r="T348" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="27" t="inlineStr">
@@ -35546,6 +36592,9 @@
       <c r="P349" s="24" t="n"/>
       <c r="Q349" s="24" t="n"/>
       <c r="R349" s="29" t="n"/>
+      <c r="T349" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="27" t="inlineStr">
@@ -35594,6 +36643,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T350" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="27" t="inlineStr">
@@ -35638,6 +36690,9 @@
       <c r="P351" s="24" t="n"/>
       <c r="Q351" s="24" t="n"/>
       <c r="R351" s="29" t="n"/>
+      <c r="T351" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="39" t="inlineStr">
@@ -35690,6 +36745,9 @@
       <c r="P352" s="41" t="n"/>
       <c r="Q352" s="41" t="n"/>
       <c r="R352" s="41" t="n"/>
+      <c r="T352" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="39" t="inlineStr">
@@ -35742,6 +36800,9 @@
       <c r="P353" s="41" t="n"/>
       <c r="Q353" s="41" t="n"/>
       <c r="R353" s="41" t="n"/>
+      <c r="T353" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="27" t="inlineStr">
@@ -35786,6 +36847,9 @@
       <c r="P354" s="24" t="n"/>
       <c r="Q354" s="24" t="n"/>
       <c r="R354" s="29" t="n"/>
+      <c r="T354" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="39" t="inlineStr">
@@ -35844,6 +36908,9 @@
       <c r="P355" s="41" t="n"/>
       <c r="Q355" s="41" t="n"/>
       <c r="R355" s="41" t="n"/>
+      <c r="T355" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="39" t="inlineStr">
@@ -35900,6 +36967,9 @@
       <c r="P356" s="41" t="n"/>
       <c r="Q356" s="41" t="n"/>
       <c r="R356" s="41" t="n"/>
+      <c r="T356" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="27" t="inlineStr">
@@ -35948,6 +37018,9 @@
           <t>I'm interested in my degree but not sure how it links to a career or the related career options.</t>
         </is>
       </c>
+      <c r="T357" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="27" t="inlineStr">
@@ -35992,6 +37065,9 @@
       <c r="P358" s="24" t="n"/>
       <c r="Q358" s="24" t="n"/>
       <c r="R358" s="29" t="n"/>
+      <c r="T358" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="27" t="inlineStr">
@@ -36036,6 +37112,9 @@
       <c r="P359" s="24" t="n"/>
       <c r="Q359" s="24" t="n"/>
       <c r="R359" s="29" t="n"/>
+      <c r="T359" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="27" t="inlineStr">
@@ -36080,6 +37159,9 @@
       <c r="P360" s="24" t="n"/>
       <c r="Q360" s="24" t="n"/>
       <c r="R360" s="29" t="n"/>
+      <c r="T360" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="27" t="inlineStr">
@@ -36124,6 +37206,9 @@
       <c r="P361" s="24" t="n"/>
       <c r="Q361" s="24" t="n"/>
       <c r="R361" s="29" t="n"/>
+      <c r="T361" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="27" t="inlineStr">
@@ -36168,6 +37253,9 @@
       <c r="P362" s="24" t="n"/>
       <c r="Q362" s="24" t="n"/>
       <c r="R362" s="29" t="n"/>
+      <c r="T362" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="27" t="inlineStr">
@@ -36212,6 +37300,9 @@
       <c r="P363" s="24" t="n"/>
       <c r="Q363" s="24" t="n"/>
       <c r="R363" s="29" t="n"/>
+      <c r="T363" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="27" t="inlineStr">
@@ -36260,6 +37351,9 @@
           <t>I’m not sure I would want a career that relates to what I am studying.</t>
         </is>
       </c>
+      <c r="T364" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="39" t="inlineStr">
@@ -36318,6 +37412,9 @@
       <c r="P365" s="41" t="n"/>
       <c r="Q365" s="41" t="n"/>
       <c r="R365" s="41" t="n"/>
+      <c r="T365" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="39" t="inlineStr">
@@ -36366,6 +37463,9 @@
       <c r="P366" s="41" t="n"/>
       <c r="Q366" s="41" t="n"/>
       <c r="R366" s="41" t="n"/>
+      <c r="T366" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="27" t="inlineStr">
@@ -36410,6 +37510,9 @@
       <c r="P367" s="24" t="n"/>
       <c r="Q367" s="24" t="n"/>
       <c r="R367" s="29" t="n"/>
+      <c r="T367" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="27" t="inlineStr">
@@ -36454,6 +37557,9 @@
       <c r="P368" s="24" t="n"/>
       <c r="Q368" s="24" t="n"/>
       <c r="R368" s="29" t="n"/>
+      <c r="T368" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="27" t="inlineStr">
@@ -36498,6 +37604,9 @@
       <c r="P369" s="24" t="n"/>
       <c r="Q369" s="24" t="n"/>
       <c r="R369" s="29" t="n"/>
+      <c r="T369" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="27" t="inlineStr">
@@ -36542,6 +37651,9 @@
       <c r="P370" s="24" t="n"/>
       <c r="Q370" s="24" t="n"/>
       <c r="R370" s="29" t="n"/>
+      <c r="T370" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="27" t="inlineStr">
@@ -36586,6 +37698,9 @@
       <c r="P371" s="24" t="n"/>
       <c r="Q371" s="24" t="n"/>
       <c r="R371" s="29" t="n"/>
+      <c r="T371" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="27" t="inlineStr">
@@ -36630,6 +37745,9 @@
       <c r="P372" s="24" t="n"/>
       <c r="Q372" s="24" t="n"/>
       <c r="R372" s="29" t="n"/>
+      <c r="T372" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="27" t="inlineStr">
@@ -36674,6 +37792,9 @@
       <c r="P373" s="24" t="n"/>
       <c r="Q373" s="24" t="n"/>
       <c r="R373" s="29" t="n"/>
+      <c r="T373" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="27" t="inlineStr">
@@ -36718,6 +37839,9 @@
       <c r="P374" s="24" t="n"/>
       <c r="Q374" s="24" t="n"/>
       <c r="R374" s="29" t="n"/>
+      <c r="T374" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="375">
       <c r="C375">
@@ -36735,6 +37859,9 @@
       <c r="M375">
         <f>SUM(M2:M374)</f>
         <v/>
+      </c>
+      <c r="T375" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>